<commit_message>
Material is exported to PDF
</commit_message>
<xml_diff>
--- a/day2/C3/excel_demo.xlsx
+++ b/day2/C3/excel_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syafribahar/Documents/gods_bootcamp03_instructors/day2/C3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF127E5-9B67-0949-BB7B-9C5E58B78053}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5ABBC6-5838-C848-AAC8-2EABDFE95111}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{E8D9986B-7092-3442-B60C-5657B6B302CD}"/>
   </bookViews>
@@ -585,307 +585,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.4004770715777379</c:v>
+                  <c:v>3.5555228365616296</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0336182704534957</c:v>
+                  <c:v>3.0984354931224463</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.379617693489062</c:v>
+                  <c:v>2.1866873843858441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9142717851697117</c:v>
+                  <c:v>3.3678136004262123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4733731458310253</c:v>
+                  <c:v>2.017641374313349</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.85254221699569699</c:v>
+                  <c:v>2.6951856700054453</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7458752718300063</c:v>
+                  <c:v>2.8636220269515178</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8573679605736324</c:v>
+                  <c:v>2.9373039276219419</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4148548321562737</c:v>
+                  <c:v>3.0246167206663341</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7978245713567205</c:v>
+                  <c:v>3.6848105866291139</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0714216313389655</c:v>
+                  <c:v>5.0612520875161993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9333610460804698</c:v>
+                  <c:v>3.2166048774370406</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8330196577717821</c:v>
+                  <c:v>3.723711017348446</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2847561458355385</c:v>
+                  <c:v>2.7602752513254414</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7697056907276032</c:v>
+                  <c:v>2.6277696169631897</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2831575616096087</c:v>
+                  <c:v>3.2415313413213971</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1951560776471353</c:v>
+                  <c:v>3.5229019587606851</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8093823939983302</c:v>
+                  <c:v>4.932174305495451</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5963307530597657</c:v>
+                  <c:v>4.1410344977812761</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1530946839495635</c:v>
+                  <c:v>4.6236236774551678</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.6528760361600776</c:v>
+                  <c:v>4.3849858097703471</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1975830501924021</c:v>
+                  <c:v>3.3963931493492518</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.700717526689504</c:v>
+                  <c:v>3.5071834186107784</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.359333391854709</c:v>
+                  <c:v>3.5929223410499693</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2964453550259847</c:v>
+                  <c:v>1.9281946035178237</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.209711169803481</c:v>
+                  <c:v>3.2440590038136663</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6312045912073723</c:v>
+                  <c:v>3.0589905867599776</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2981581193932676</c:v>
+                  <c:v>3.93486476991851</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.6855131915015302</c:v>
+                  <c:v>2.6274656913171035</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2394720874267104</c:v>
+                  <c:v>3.3365416967764578</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.71038747533669566</c:v>
+                  <c:v>2.3675563570112663</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.9146629754045792</c:v>
+                  <c:v>4.3059341237087674</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.1309188477513183</c:v>
+                  <c:v>2.9780177310684457</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3370686958884779</c:v>
+                  <c:v>4.7568911152041746</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.7404500568578407</c:v>
+                  <c:v>3.574999864529961</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.674128781037961</c:v>
+                  <c:v>2.4549422676790589</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.8228882563197456</c:v>
+                  <c:v>2.2176396743841074</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.1023502890887507</c:v>
+                  <c:v>4.9143535800073632</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1811757535330845</c:v>
+                  <c:v>2.944955108082282</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.3492025905797616</c:v>
+                  <c:v>2.9994081348178598</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.7264453371085859</c:v>
+                  <c:v>5.2350484283745953</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.3928245518877729</c:v>
+                  <c:v>3.199569319045104</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.2575568864417885</c:v>
+                  <c:v>4.3568904041731145</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.4979160238618432</c:v>
+                  <c:v>2.8583029111785221</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.8216249993318463</c:v>
+                  <c:v>2.6723054753488595</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.3731797218350343</c:v>
+                  <c:v>5.0365593757108478</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.17381618739152</c:v>
+                  <c:v>2.4659395127891317</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.2287231060616874</c:v>
+                  <c:v>4.3337873958886348</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.975989167075606</c:v>
+                  <c:v>3.6760056493564539</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.9089438198659074</c:v>
+                  <c:v>4.5186949803790624</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.7516103811452775</c:v>
+                  <c:v>4.1609660701205282</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.9672479391857371</c:v>
+                  <c:v>2.5556196803345737</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.3887703037903836</c:v>
+                  <c:v>3.9089619562854785</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.1149221137813252</c:v>
+                  <c:v>3.7678810073494642</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.2793914856477053</c:v>
+                  <c:v>2.0376619150557969</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.4753879648283021</c:v>
+                  <c:v>2.8450845287731914</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.2291514716753413</c:v>
+                  <c:v>3.0643690278876319</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.4887251341899308</c:v>
+                  <c:v>2.5711298082411096</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.7563502148388754</c:v>
+                  <c:v>3.7373762427002193</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.2887531876147142</c:v>
+                  <c:v>2.9697919812250104</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.0132980511482983</c:v>
+                  <c:v>3.3842735068159828</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.9748623817434736</c:v>
+                  <c:v>4.4630017897230152</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.2586570354220332</c:v>
+                  <c:v>3.0843256662644527</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.4178083220778221</c:v>
+                  <c:v>3.9357020629991788</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.99426722135127876</c:v>
+                  <c:v>2.816576469786936</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.0223336523907784</c:v>
+                  <c:v>5.1495894664162929</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.91817399156036639</c:v>
+                  <c:v>2.3555770332498627</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.5579361063075159</c:v>
+                  <c:v>2.0417020148554208</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.5774395275798039</c:v>
+                  <c:v>3.7906128355760309</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.5868906503056226</c:v>
+                  <c:v>3.701311791000971</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.0098205837981467</c:v>
+                  <c:v>4.9785801930770619</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.9323267729229716</c:v>
+                  <c:v>3.3389587469668935</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.78548816263778676</c:v>
+                  <c:v>2.4709245565001225</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.9364247999189663</c:v>
+                  <c:v>3.1203683938119946</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.7845275489471808</c:v>
+                  <c:v>3.7558504471257343</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.2292509305092356</c:v>
+                  <c:v>1.8334733976489672</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2.2156171510316578</c:v>
+                  <c:v>3.5558885543926007</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2.6277491886100512</c:v>
+                  <c:v>4.0738972555715023</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.7390240397019165</c:v>
+                  <c:v>2.2187159817317172</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.2749522009181147</c:v>
+                  <c:v>2.8024768107579519</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.9714767074245687</c:v>
+                  <c:v>4.2369418479217806</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.4878904624125808</c:v>
+                  <c:v>2.1748360615976829</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.5382322063238609</c:v>
+                  <c:v>4.3310112688230502</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2.4485851925293947</c:v>
+                  <c:v>3.702980823783756</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.98002518204360289</c:v>
+                  <c:v>2.2089726215871872</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.5919945431773663</c:v>
+                  <c:v>2.742795921918634</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.1097096612682154</c:v>
+                  <c:v>2.0371932610723045</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.3527612837761769</c:v>
+                  <c:v>2.4762665406416984</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.89994584158051771</c:v>
+                  <c:v>1.8970726836200043</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.195589871554203</c:v>
+                  <c:v>2.7962043022396905</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.7247555825518095</c:v>
+                  <c:v>4.2804187806988239</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3.3218993466617333</c:v>
+                  <c:v>4.7193093010875211</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.521767643570723</c:v>
+                  <c:v>4.8040007665895113</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.3741398457741898</c:v>
+                  <c:v>5.0258685688349276</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2.2208922914881963</c:v>
+                  <c:v>4.7121649678001694</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.3393404507427444</c:v>
+                  <c:v>2.4250178195836805</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.3607825536926208</c:v>
+                  <c:v>2.4891353916696941</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.3386551978926224</c:v>
+                  <c:v>2.3467148217234914</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.66098871815761362</c:v>
+                  <c:v>1.7964776317093307</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0843316607618232</c:v>
+                  <c:v>3.1883951077693222</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.2044447586154736</c:v>
+                  <c:v>2.3008262150147778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -30563,7 +30563,7 @@
   <dimension ref="B1:F107"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30578,7 +30578,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -30586,7 +30586,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -30611,7 +30611,7 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" ref="C7:C38" ca="1" si="0">$C$2*B7+$C$3+$C$4*(2*RAND()-1)</f>
-        <v>1.4004770715777379</v>
+        <v>3.5555228365616296</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -30620,7 +30620,7 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0336182704534957</v>
+        <v>3.0984354931224463</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -30629,7 +30629,7 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.379617693489062</v>
+        <v>2.1866873843858441</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -30638,7 +30638,7 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9142717851697117</v>
+        <v>3.3678136004262123</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -30649,7 +30649,7 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4733731458310253</v>
+        <v>2.017641374313349</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -30658,7 +30658,7 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85254221699569699</v>
+        <v>2.6951856700054453</v>
       </c>
     </row>
     <row r="13" spans="2:6">
@@ -30667,7 +30667,7 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7458752718300063</v>
+        <v>2.8636220269515178</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -30676,7 +30676,7 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8573679605736324</v>
+        <v>2.9373039276219419</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -30685,7 +30685,7 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4148548321562737</v>
+        <v>3.0246167206663341</v>
       </c>
     </row>
     <row r="16" spans="2:6">
@@ -30694,7 +30694,7 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7978245713567205</v>
+        <v>3.6848105866291139</v>
       </c>
     </row>
     <row r="17" spans="2:3">
@@ -30703,7 +30703,7 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0714216313389655</v>
+        <v>5.0612520875161993</v>
       </c>
     </row>
     <row r="18" spans="2:3">
@@ -30712,7 +30712,7 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9333610460804698</v>
+        <v>3.2166048774370406</v>
       </c>
     </row>
     <row r="19" spans="2:3">
@@ -30721,7 +30721,7 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8330196577717821</v>
+        <v>3.723711017348446</v>
       </c>
     </row>
     <row r="20" spans="2:3">
@@ -30730,7 +30730,7 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2847561458355385</v>
+        <v>2.7602752513254414</v>
       </c>
     </row>
     <row r="21" spans="2:3">
@@ -30739,7 +30739,7 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7697056907276032</v>
+        <v>2.6277696169631897</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -30748,7 +30748,7 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2831575616096087</v>
+        <v>3.2415313413213971</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -30757,7 +30757,7 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1951560776471353</v>
+        <v>3.5229019587606851</v>
       </c>
     </row>
     <row r="24" spans="2:3">
@@ -30766,7 +30766,7 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8093823939983302</v>
+        <v>4.932174305495451</v>
       </c>
     </row>
     <row r="25" spans="2:3">
@@ -30775,7 +30775,7 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5963307530597657</v>
+        <v>4.1410344977812761</v>
       </c>
     </row>
     <row r="26" spans="2:3">
@@ -30784,7 +30784,7 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1530946839495635</v>
+        <v>4.6236236774551678</v>
       </c>
     </row>
     <row r="27" spans="2:3">
@@ -30793,7 +30793,7 @@
       </c>
       <c r="C27" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6528760361600776</v>
+        <v>4.3849858097703471</v>
       </c>
     </row>
     <row r="28" spans="2:3">
@@ -30802,7 +30802,7 @@
       </c>
       <c r="C28" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1975830501924021</v>
+        <v>3.3963931493492518</v>
       </c>
     </row>
     <row r="29" spans="2:3">
@@ -30811,7 +30811,7 @@
       </c>
       <c r="C29" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.700717526689504</v>
+        <v>3.5071834186107784</v>
       </c>
     </row>
     <row r="30" spans="2:3">
@@ -30820,7 +30820,7 @@
       </c>
       <c r="C30" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.359333391854709</v>
+        <v>3.5929223410499693</v>
       </c>
     </row>
     <row r="31" spans="2:3">
@@ -30829,7 +30829,7 @@
       </c>
       <c r="C31" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2964453550259847</v>
+        <v>1.9281946035178237</v>
       </c>
     </row>
     <row r="32" spans="2:3">
@@ -30838,7 +30838,7 @@
       </c>
       <c r="C32" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.209711169803481</v>
+        <v>3.2440590038136663</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -30847,7 +30847,7 @@
       </c>
       <c r="C33" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6312045912073723</v>
+        <v>3.0589905867599776</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -30856,7 +30856,7 @@
       </c>
       <c r="C34" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2981581193932676</v>
+        <v>3.93486476991851</v>
       </c>
     </row>
     <row r="35" spans="2:3">
@@ -30865,7 +30865,7 @@
       </c>
       <c r="C35" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6855131915015302</v>
+        <v>2.6274656913171035</v>
       </c>
     </row>
     <row r="36" spans="2:3">
@@ -30874,7 +30874,7 @@
       </c>
       <c r="C36" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2394720874267104</v>
+        <v>3.3365416967764578</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -30883,7 +30883,7 @@
       </c>
       <c r="C37" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71038747533669566</v>
+        <v>2.3675563570112663</v>
       </c>
     </row>
     <row r="38" spans="2:3">
@@ -30892,7 +30892,7 @@
       </c>
       <c r="C38" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9146629754045792</v>
+        <v>4.3059341237087674</v>
       </c>
     </row>
     <row r="39" spans="2:3">
@@ -30901,7 +30901,7 @@
       </c>
       <c r="C39" s="3">
         <f t="shared" ref="C39:C70" ca="1" si="1">$C$2*B39+$C$3+$C$4*(2*RAND()-1)</f>
-        <v>1.1309188477513183</v>
+        <v>2.9780177310684457</v>
       </c>
     </row>
     <row r="40" spans="2:3">
@@ -30910,7 +30910,7 @@
       </c>
       <c r="C40" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3370686958884779</v>
+        <v>4.7568911152041746</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -30919,7 +30919,7 @@
       </c>
       <c r="C41" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7404500568578407</v>
+        <v>3.574999864529961</v>
       </c>
     </row>
     <row r="42" spans="2:3">
@@ -30928,7 +30928,7 @@
       </c>
       <c r="C42" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.674128781037961</v>
+        <v>2.4549422676790589</v>
       </c>
     </row>
     <row r="43" spans="2:3">
@@ -30937,7 +30937,7 @@
       </c>
       <c r="C43" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8228882563197456</v>
+        <v>2.2176396743841074</v>
       </c>
     </row>
     <row r="44" spans="2:3">
@@ -30946,7 +30946,7 @@
       </c>
       <c r="C44" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1023502890887507</v>
+        <v>4.9143535800073632</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -30955,7 +30955,7 @@
       </c>
       <c r="C45" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1811757535330845</v>
+        <v>2.944955108082282</v>
       </c>
     </row>
     <row r="46" spans="2:3">
@@ -30964,7 +30964,7 @@
       </c>
       <c r="C46" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3492025905797616</v>
+        <v>2.9994081348178598</v>
       </c>
     </row>
     <row r="47" spans="2:3">
@@ -30973,7 +30973,7 @@
       </c>
       <c r="C47" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7264453371085859</v>
+        <v>5.2350484283745953</v>
       </c>
     </row>
     <row r="48" spans="2:3">
@@ -30982,7 +30982,7 @@
       </c>
       <c r="C48" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3928245518877729</v>
+        <v>3.199569319045104</v>
       </c>
     </row>
     <row r="49" spans="2:3">
@@ -30991,7 +30991,7 @@
       </c>
       <c r="C49" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2575568864417885</v>
+        <v>4.3568904041731145</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -31000,7 +31000,7 @@
       </c>
       <c r="C50" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4979160238618432</v>
+        <v>2.8583029111785221</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -31009,7 +31009,7 @@
       </c>
       <c r="C51" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8216249993318463</v>
+        <v>2.6723054753488595</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -31018,7 +31018,7 @@
       </c>
       <c r="C52" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3731797218350343</v>
+        <v>5.0365593757108478</v>
       </c>
     </row>
     <row r="53" spans="2:3">
@@ -31027,7 +31027,7 @@
       </c>
       <c r="C53" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.17381618739152</v>
+        <v>2.4659395127891317</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -31036,7 +31036,7 @@
       </c>
       <c r="C54" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2287231060616874</v>
+        <v>4.3337873958886348</v>
       </c>
     </row>
     <row r="55" spans="2:3">
@@ -31045,7 +31045,7 @@
       </c>
       <c r="C55" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.975989167075606</v>
+        <v>3.6760056493564539</v>
       </c>
     </row>
     <row r="56" spans="2:3">
@@ -31054,7 +31054,7 @@
       </c>
       <c r="C56" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9089438198659074</v>
+        <v>4.5186949803790624</v>
       </c>
     </row>
     <row r="57" spans="2:3">
@@ -31063,7 +31063,7 @@
       </c>
       <c r="C57" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7516103811452775</v>
+        <v>4.1609660701205282</v>
       </c>
     </row>
     <row r="58" spans="2:3">
@@ -31072,7 +31072,7 @@
       </c>
       <c r="C58" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9672479391857371</v>
+        <v>2.5556196803345737</v>
       </c>
     </row>
     <row r="59" spans="2:3">
@@ -31081,7 +31081,7 @@
       </c>
       <c r="C59" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3887703037903836</v>
+        <v>3.9089619562854785</v>
       </c>
     </row>
     <row r="60" spans="2:3">
@@ -31090,7 +31090,7 @@
       </c>
       <c r="C60" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1149221137813252</v>
+        <v>3.7678810073494642</v>
       </c>
     </row>
     <row r="61" spans="2:3">
@@ -31099,7 +31099,7 @@
       </c>
       <c r="C61" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2793914856477053</v>
+        <v>2.0376619150557969</v>
       </c>
     </row>
     <row r="62" spans="2:3">
@@ -31108,7 +31108,7 @@
       </c>
       <c r="C62" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4753879648283021</v>
+        <v>2.8450845287731914</v>
       </c>
     </row>
     <row r="63" spans="2:3">
@@ -31117,7 +31117,7 @@
       </c>
       <c r="C63" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2291514716753413</v>
+        <v>3.0643690278876319</v>
       </c>
     </row>
     <row r="64" spans="2:3">
@@ -31126,7 +31126,7 @@
       </c>
       <c r="C64" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4887251341899308</v>
+        <v>2.5711298082411096</v>
       </c>
     </row>
     <row r="65" spans="2:3">
@@ -31135,7 +31135,7 @@
       </c>
       <c r="C65" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7563502148388754</v>
+        <v>3.7373762427002193</v>
       </c>
     </row>
     <row r="66" spans="2:3">
@@ -31144,7 +31144,7 @@
       </c>
       <c r="C66" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2887531876147142</v>
+        <v>2.9697919812250104</v>
       </c>
     </row>
     <row r="67" spans="2:3">
@@ -31153,7 +31153,7 @@
       </c>
       <c r="C67" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0132980511482983</v>
+        <v>3.3842735068159828</v>
       </c>
     </row>
     <row r="68" spans="2:3">
@@ -31162,7 +31162,7 @@
       </c>
       <c r="C68" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9748623817434736</v>
+        <v>4.4630017897230152</v>
       </c>
     </row>
     <row r="69" spans="2:3">
@@ -31171,7 +31171,7 @@
       </c>
       <c r="C69" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2586570354220332</v>
+        <v>3.0843256662644527</v>
       </c>
     </row>
     <row r="70" spans="2:3">
@@ -31180,7 +31180,7 @@
       </c>
       <c r="C70" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4178083220778221</v>
+        <v>3.9357020629991788</v>
       </c>
     </row>
     <row r="71" spans="2:3">
@@ -31189,7 +31189,7 @@
       </c>
       <c r="C71" s="3">
         <f t="shared" ref="C71:C102" ca="1" si="2">$C$2*B71+$C$3+$C$4*(2*RAND()-1)</f>
-        <v>0.99426722135127876</v>
+        <v>2.816576469786936</v>
       </c>
     </row>
     <row r="72" spans="2:3">
@@ -31198,7 +31198,7 @@
       </c>
       <c r="C72" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0223336523907784</v>
+        <v>5.1495894664162929</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -31207,7 +31207,7 @@
       </c>
       <c r="C73" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.91817399156036639</v>
+        <v>2.3555770332498627</v>
       </c>
     </row>
     <row r="74" spans="2:3">
@@ -31216,7 +31216,7 @@
       </c>
       <c r="C74" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5579361063075159</v>
+        <v>2.0417020148554208</v>
       </c>
     </row>
     <row r="75" spans="2:3">
@@ -31225,7 +31225,7 @@
       </c>
       <c r="C75" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5774395275798039</v>
+        <v>3.7906128355760309</v>
       </c>
     </row>
     <row r="76" spans="2:3">
@@ -31234,7 +31234,7 @@
       </c>
       <c r="C76" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5868906503056226</v>
+        <v>3.701311791000971</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -31243,7 +31243,7 @@
       </c>
       <c r="C77" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0098205837981467</v>
+        <v>4.9785801930770619</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -31252,7 +31252,7 @@
       </c>
       <c r="C78" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9323267729229716</v>
+        <v>3.3389587469668935</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -31261,7 +31261,7 @@
       </c>
       <c r="C79" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.78548816263778676</v>
+        <v>2.4709245565001225</v>
       </c>
     </row>
     <row r="80" spans="2:3">
@@ -31270,7 +31270,7 @@
       </c>
       <c r="C80" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9364247999189663</v>
+        <v>3.1203683938119946</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -31279,7 +31279,7 @@
       </c>
       <c r="C81" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7845275489471808</v>
+        <v>3.7558504471257343</v>
       </c>
     </row>
     <row r="82" spans="2:3">
@@ -31288,7 +31288,7 @@
       </c>
       <c r="C82" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2292509305092356</v>
+        <v>1.8334733976489672</v>
       </c>
     </row>
     <row r="83" spans="2:3">
@@ -31297,7 +31297,7 @@
       </c>
       <c r="C83" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2156171510316578</v>
+        <v>3.5558885543926007</v>
       </c>
     </row>
     <row r="84" spans="2:3">
@@ -31306,7 +31306,7 @@
       </c>
       <c r="C84" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6277491886100512</v>
+        <v>4.0738972555715023</v>
       </c>
     </row>
     <row r="85" spans="2:3">
@@ -31315,7 +31315,7 @@
       </c>
       <c r="C85" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7390240397019165</v>
+        <v>2.2187159817317172</v>
       </c>
     </row>
     <row r="86" spans="2:3">
@@ -31324,7 +31324,7 @@
       </c>
       <c r="C86" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2749522009181147</v>
+        <v>2.8024768107579519</v>
       </c>
     </row>
     <row r="87" spans="2:3">
@@ -31333,7 +31333,7 @@
       </c>
       <c r="C87" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9714767074245687</v>
+        <v>4.2369418479217806</v>
       </c>
     </row>
     <row r="88" spans="2:3">
@@ -31342,7 +31342,7 @@
       </c>
       <c r="C88" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4878904624125808</v>
+        <v>2.1748360615976829</v>
       </c>
     </row>
     <row r="89" spans="2:3">
@@ -31351,7 +31351,7 @@
       </c>
       <c r="C89" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5382322063238609</v>
+        <v>4.3310112688230502</v>
       </c>
     </row>
     <row r="90" spans="2:3">
@@ -31360,7 +31360,7 @@
       </c>
       <c r="C90" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4485851925293947</v>
+        <v>3.702980823783756</v>
       </c>
     </row>
     <row r="91" spans="2:3">
@@ -31369,7 +31369,7 @@
       </c>
       <c r="C91" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.98002518204360289</v>
+        <v>2.2089726215871872</v>
       </c>
     </row>
     <row r="92" spans="2:3">
@@ -31378,7 +31378,7 @@
       </c>
       <c r="C92" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5919945431773663</v>
+        <v>2.742795921918634</v>
       </c>
     </row>
     <row r="93" spans="2:3">
@@ -31387,7 +31387,7 @@
       </c>
       <c r="C93" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1097096612682154</v>
+        <v>2.0371932610723045</v>
       </c>
     </row>
     <row r="94" spans="2:3">
@@ -31396,7 +31396,7 @@
       </c>
       <c r="C94" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3527612837761769</v>
+        <v>2.4762665406416984</v>
       </c>
     </row>
     <row r="95" spans="2:3">
@@ -31405,7 +31405,7 @@
       </c>
       <c r="C95" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89994584158051771</v>
+        <v>1.8970726836200043</v>
       </c>
     </row>
     <row r="96" spans="2:3">
@@ -31414,7 +31414,7 @@
       </c>
       <c r="C96" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.195589871554203</v>
+        <v>2.7962043022396905</v>
       </c>
     </row>
     <row r="97" spans="2:3">
@@ -31423,7 +31423,7 @@
       </c>
       <c r="C97" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7247555825518095</v>
+        <v>4.2804187806988239</v>
       </c>
     </row>
     <row r="98" spans="2:3">
@@ -31432,7 +31432,7 @@
       </c>
       <c r="C98" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3218993466617333</v>
+        <v>4.7193093010875211</v>
       </c>
     </row>
     <row r="99" spans="2:3">
@@ -31441,7 +31441,7 @@
       </c>
       <c r="C99" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.521767643570723</v>
+        <v>4.8040007665895113</v>
       </c>
     </row>
     <row r="100" spans="2:3">
@@ -31450,7 +31450,7 @@
       </c>
       <c r="C100" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.3741398457741898</v>
+        <v>5.0258685688349276</v>
       </c>
     </row>
     <row r="101" spans="2:3">
@@ -31459,7 +31459,7 @@
       </c>
       <c r="C101" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2208922914881963</v>
+        <v>4.7121649678001694</v>
       </c>
     </row>
     <row r="102" spans="2:3">
@@ -31468,7 +31468,7 @@
       </c>
       <c r="C102" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3393404507427444</v>
+        <v>2.4250178195836805</v>
       </c>
     </row>
     <row r="103" spans="2:3">
@@ -31476,8 +31476,8 @@
         <v>0.21070429792126311</v>
       </c>
       <c r="C103" s="3">
-        <f t="shared" ref="C103:C134" ca="1" si="3">$C$2*B103+$C$3+$C$4*(2*RAND()-1)</f>
-        <v>1.3607825536926208</v>
+        <f t="shared" ref="C103:C107" ca="1" si="3">$C$2*B103+$C$3+$C$4*(2*RAND()-1)</f>
+        <v>2.4891353916696941</v>
       </c>
     </row>
     <row r="104" spans="2:3">
@@ -31486,7 +31486,7 @@
       </c>
       <c r="C104" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3386551978926224</v>
+        <v>2.3467148217234914</v>
       </c>
     </row>
     <row r="105" spans="2:3">
@@ -31495,7 +31495,7 @@
       </c>
       <c r="C105" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.66098871815761362</v>
+        <v>1.7964776317093307</v>
       </c>
     </row>
     <row r="106" spans="2:3">
@@ -31504,7 +31504,7 @@
       </c>
       <c r="C106" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0843316607618232</v>
+        <v>3.1883951077693222</v>
       </c>
     </row>
     <row r="107" spans="2:3">
@@ -31513,7 +31513,7 @@
       </c>
       <c r="C107" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2044447586154736</v>
+        <v>2.3008262150147778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>